<commit_message>
param param tes tes
</commit_message>
<xml_diff>
--- a/tabel_hasil_percobaan.xlsx
+++ b/tabel_hasil_percobaan.xlsx
@@ -24,39 +24,74 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="8">
-  <si>
-    <t>Lexical</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
   <si>
     <t>SVM</t>
   </si>
   <si>
-    <t>Naïve Bayes</t>
-  </si>
-  <si>
-    <t>Stemming</t>
-  </si>
-  <si>
-    <t>Lemmatization</t>
-  </si>
-  <si>
-    <t>Accuracy</t>
-  </si>
-  <si>
-    <t>x</t>
-  </si>
-  <si>
-    <t>v</t>
+    <t>Rule based</t>
+  </si>
+  <si>
+    <t>Decision tree</t>
+  </si>
+  <si>
+    <t>Naïve bayes</t>
+  </si>
+  <si>
+    <t>Random forest</t>
+  </si>
+  <si>
+    <t>Neural network</t>
+  </si>
+  <si>
+    <t>Vector space model</t>
+  </si>
+  <si>
+    <t>KNN</t>
+  </si>
+  <si>
+    <t>SGD</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>TEST DATA = TEST DATA</t>
+  </si>
+  <si>
+    <t>TEST DATA = TRAINING DATA</t>
+  </si>
+  <si>
+    <t>Combinations</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -71,7 +106,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -79,12 +114,42 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -365,135 +430,232 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" style="1"/>
+    <col min="3" max="3" width="8.77734375" style="1" customWidth="1"/>
+    <col min="4" max="11" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B1" t="s">
+    <row r="1" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="3"/>
+      <c r="B1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+    </row>
+    <row r="2" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="7">
+        <v>0.77</v>
+      </c>
+      <c r="C3" s="7">
+        <v>0.878</v>
+      </c>
+      <c r="D3" s="7">
+        <v>0.878</v>
+      </c>
+      <c r="E3" s="7">
+        <v>0.86399999999999999</v>
+      </c>
+      <c r="F3" s="7">
+        <v>0.90500000000000003</v>
+      </c>
+      <c r="G3" s="7">
+        <v>0.997</v>
+      </c>
+      <c r="H3" s="7">
+        <v>0.998</v>
+      </c>
+      <c r="I3" s="7">
+        <v>0.998</v>
+      </c>
+      <c r="J3" s="7">
+        <v>0.998</v>
+      </c>
+      <c r="K3" s="7">
+        <v>0.998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D2">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3">
-        <v>98.04</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>1</v>
-      </c>
-      <c r="B9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" t="s">
-        <v>7</v>
-      </c>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="G1:K1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>